<commit_message>
Fix dark mode text visibility and show full document content
</commit_message>
<xml_diff>
--- a/docs/Test_Cases_Document.xlsx
+++ b/docs/Test_Cases_Document.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adity\OneDrive\Desktop\azure-ai-search-portal\azure-ai-search-portal\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844CA147-37DA-47F9-A830-BE1FB6493EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8784E22-0C3D-4178-8215-A8E93838383E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -561,10 +561,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -871,7 +877,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -896,7 +902,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -922,7 +928,7 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>1</v>
       </c>
       <c r="E2" t="s">
@@ -948,7 +954,7 @@
       <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
@@ -974,7 +980,7 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>3</v>
       </c>
       <c r="E4" t="s">
@@ -1000,7 +1006,7 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>4</v>
       </c>
       <c r="E5" t="s">
@@ -1026,7 +1032,7 @@
       <c r="C6" t="s">
         <v>35</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>5</v>
       </c>
       <c r="E6" t="s">
@@ -1052,7 +1058,7 @@
       <c r="C7" t="s">
         <v>35</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>6</v>
       </c>
       <c r="E7" t="s">
@@ -1078,7 +1084,7 @@
       <c r="C8" t="s">
         <v>35</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>7</v>
       </c>
       <c r="E8" t="s">
@@ -1104,7 +1110,7 @@
       <c r="C9" t="s">
         <v>35</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>8</v>
       </c>
       <c r="E9" t="s">
@@ -1130,7 +1136,7 @@
       <c r="C10" t="s">
         <v>35</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>9</v>
       </c>
       <c r="E10" t="s">
@@ -1156,7 +1162,7 @@
       <c r="C11" t="s">
         <v>35</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>10</v>
       </c>
       <c r="E11" t="s">
@@ -1182,7 +1188,7 @@
       <c r="C12" t="s">
         <v>72</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <v>11</v>
       </c>
       <c r="E12" t="s">
@@ -1208,7 +1214,7 @@
       <c r="C13" t="s">
         <v>72</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>12</v>
       </c>
       <c r="E13" t="s">
@@ -1234,7 +1240,7 @@
       <c r="C14" t="s">
         <v>17</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
         <v>13</v>
       </c>
       <c r="E14" t="s">
@@ -1260,7 +1266,7 @@
       <c r="C15" t="s">
         <v>90</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>14</v>
       </c>
       <c r="E15" t="s">
@@ -1286,7 +1292,7 @@
       <c r="C16" t="s">
         <v>90</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>15</v>
       </c>
       <c r="E16" t="s">
@@ -1312,7 +1318,7 @@
       <c r="C17" t="s">
         <v>102</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="3">
         <v>16</v>
       </c>
       <c r="E17" t="s">
@@ -1338,7 +1344,7 @@
       <c r="C18" t="s">
         <v>102</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="3">
         <v>17</v>
       </c>
       <c r="E18" t="s">
@@ -1364,7 +1370,7 @@
       <c r="C19" t="s">
         <v>102</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="3">
         <v>18</v>
       </c>
       <c r="E19" t="s">
@@ -1390,7 +1396,7 @@
       <c r="C20" t="s">
         <v>10</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <v>19</v>
       </c>
       <c r="E20" t="s">
@@ -1416,7 +1422,7 @@
       <c r="C21" t="s">
         <v>127</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="3">
         <v>20</v>
       </c>
       <c r="E21" t="s">
@@ -1442,7 +1448,7 @@
       <c r="C22" t="s">
         <v>127</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="3">
         <v>21</v>
       </c>
       <c r="E22" t="s">
@@ -1468,7 +1474,7 @@
       <c r="C23" t="s">
         <v>140</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
         <v>22</v>
       </c>
       <c r="E23" t="s">
@@ -1494,7 +1500,7 @@
       <c r="C24" t="s">
         <v>140</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="3">
         <v>23</v>
       </c>
       <c r="E24" t="s">
@@ -1520,7 +1526,7 @@
       <c r="C25" t="s">
         <v>150</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="3">
         <v>24</v>
       </c>
       <c r="E25" t="s">
@@ -1546,7 +1552,7 @@
       <c r="C26" t="s">
         <v>157</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="3">
         <v>25</v>
       </c>
       <c r="E26" t="s">

</xml_diff>